<commit_message>
updated mapping file based on 2/20 meeting with David
</commit_message>
<xml_diff>
--- a/documents/vMR_QDM_ComparisonMatrix.xlsx
+++ b/documents/vMR_QDM_ComparisonMatrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="20010" windowHeight="7605" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="20010" windowHeight="7605" firstSheet="13" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="656">
   <si>
     <t>//element(*,VMR)/patient/clinicalStatements/adverseEvents/adverseEvent</t>
   </si>
@@ -2000,13 +2000,25 @@
   </si>
   <si>
     <t>EncounterEvent with a related Facility [with code for facility type] having relationship code for types of transfer (billing codes)</t>
+  </si>
+  <si>
+    <t>Dose (?) Unsure</t>
+  </si>
+  <si>
+    <t>RTO (SHOULD BE RTO_PQ)</t>
+  </si>
+  <si>
+    <t>No equivalent unless precoordinated or within dose (?)</t>
+  </si>
+  <si>
+    <t>May be precoordinated in term</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2027,6 +2039,13 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2052,7 +2071,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2077,6 +2096,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3011,9 +3031,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3102,7 +3122,7 @@
         <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>433</v>
+        <v>652</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3158,11 +3178,11 @@
       <c r="A13" t="s">
         <v>128</v>
       </c>
-      <c r="B13" t="s">
-        <v>143</v>
+      <c r="B13" s="10" t="s">
+        <v>653</v>
       </c>
       <c r="E13" t="s">
-        <v>539</v>
+        <v>580</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -3173,7 +3193,7 @@
         <v>44</v>
       </c>
       <c r="E14" t="s">
-        <v>433</v>
+        <v>654</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -3195,7 +3215,7 @@
         <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>433</v>
+        <v>655</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -4489,7 +4509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A50" workbookViewId="0">
       <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
@@ -6566,7 +6586,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>556</v>
       </c>

</xml_diff>